<commit_message>
ajout des figures e- au rapport dosi relative
</commit_message>
<xml_diff>
--- a/RT4/export_excel/profils.xlsx
+++ b/RT4/export_excel/profils.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/LEXAR/Fiches_DQ/RT/RT4/export_excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08499C71-8FBC-7A48-80AD-28A69AE0635B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9D29F59-4B4B-614D-BFB4-D01741D0D5EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16360" activeTab="3" xr2:uid="{6567EACF-C6A6-244B-9A4A-E489798AB033}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16360" firstSheet="11" activeTab="14" xr2:uid="{6567EACF-C6A6-244B-9A4A-E489798AB033}"/>
   </bookViews>
   <sheets>
     <sheet name="IN_06MeV_10_DSP100_CC13" sheetId="10" r:id="rId1"/>
@@ -27,7 +27,7 @@
     <sheet name="CR_09MeV_10_DSP100_CC13_rap" sheetId="13" r:id="rId12"/>
     <sheet name="CR_09MeV_10_DSP105_CC13" sheetId="14" r:id="rId13"/>
     <sheet name="CR_09MeV_10_DSP110_CC13" sheetId="15" r:id="rId14"/>
-    <sheet name="CR_09MeV_6_DSP100_CC13" sheetId="16" r:id="rId15"/>
+    <sheet name="CR_09MeV_06_DSP100_CC13" sheetId="16" r:id="rId15"/>
     <sheet name="CR_09MeV_15_DSP100_CC13" sheetId="17" r:id="rId16"/>
     <sheet name="CR_09MeV_20_DSP100_CC13" sheetId="18" r:id="rId17"/>
     <sheet name="IN_09MeV_10_DSP100_ROOS" sheetId="19" r:id="rId18"/>
@@ -14389,7 +14389,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CAC9518-5A57-0C4C-8DC9-4998740D8C3C}">
   <dimension ref="A1:B254"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:B254"/>
     </sheetView>
   </sheetViews>
@@ -31606,7 +31606,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5AEE371-FB0D-2E41-B337-E2AFD5E0FC65}">
   <dimension ref="A1:B287"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>

</xml_diff>